<commit_message>
Data Driven Tests using CSV
</commit_message>
<xml_diff>
--- a/TestData/TestDataRobot.xlsx
+++ b/TestData/TestDataRobot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\savig\PycharmProjects\PythonProject\.venv\testcases\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEA9DAE8-69C5-4B2C-8CA6-7AC371DD3FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AEDBEFC-F02E-428A-A62E-81B3388ABBA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3840" yWindow="3408" windowWidth="17280" windowHeight="8964" xr2:uid="{F3B539F4-4805-4758-B5D5-26C5B2154C4D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>${username}</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>Admin1</t>
+  </si>
+  <si>
+    <t>1231@yopmail.com</t>
+  </si>
+  <si>
+    <t>adm1</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,10 +487,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>